<commit_message>
Second Commit, updated results excel file and libraries folder
</commit_message>
<xml_diff>
--- a/DDAS.Selenium/Testing_Results.xlsx
+++ b/DDAS.Selenium/Testing_Results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t>URL</t>
   </si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t>Has a search box. Last name and first name</t>
-  </si>
-  <si>
-    <t>Has a search box, class and functions are aleady in place. Need to code for initial search parameters</t>
   </si>
   <si>
     <t>Y</t>
@@ -177,7 +174,7 @@
     <t>David Freeman</t>
   </si>
   <si>
-    <t>Need to find multiple occurances of the names in each of the websites and provide a Json result</t>
+    <t>Has a search box</t>
   </si>
 </sst>
 </file>
@@ -625,8 +622,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,20 +649,20 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -676,20 +673,18 @@
         <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1">
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -700,19 +695,19 @@
         <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="F3" s="1">
         <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -724,10 +719,10 @@
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -744,14 +739,14 @@
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1">
         <v>9</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H5" s="13"/>
     </row>
@@ -766,14 +761,14 @@
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1">
         <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H6" s="13"/>
     </row>
@@ -788,14 +783,14 @@
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1">
         <v>7</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H7" s="13"/>
     </row>
@@ -810,14 +805,14 @@
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
         <v>51</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H8" s="13"/>
     </row>
@@ -832,7 +827,7 @@
         <v>29</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>31</v>
@@ -852,7 +847,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>32</v>
@@ -861,10 +856,10 @@
         <v>124</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -875,7 +870,7 @@
         <v>25</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>30</v>
@@ -893,7 +888,7 @@
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>30</v>
@@ -913,16 +908,16 @@
         <v>4</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" s="1">
         <v>56</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H13" s="13"/>
     </row>
@@ -964,15 +959,15 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Search Function for all the sites (Except the ones that have some queries). Able to get Json result for all sites
</commit_message>
<xml_diff>
--- a/DDAS.Selenium/Testing_Results.xlsx
+++ b/DDAS.Selenium/Testing_Results.xlsx
@@ -4,23 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DDAS" sheetId="1" r:id="rId1"/>
     <sheet name="SearchEngine" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Log" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Log!$A$1:$E$1148</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SearchEngine!$A$1:$E$1148</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$A$1:$E$1148</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t>URL</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Next Task</t>
   </si>
   <si>
-    <t>Update LoadContents function</t>
-  </si>
-  <si>
     <t>Input Names</t>
   </si>
   <si>
@@ -175,6 +172,30 @@
   </si>
   <si>
     <t>Has a search box</t>
+  </si>
+  <si>
+    <t>Working copy path:</t>
+  </si>
+  <si>
+    <t>C:\Development\p926-ddas</t>
+  </si>
+  <si>
+    <t>Files Updated</t>
+  </si>
+  <si>
+    <t>Files Created</t>
+  </si>
+  <si>
+    <t>Context updated</t>
+  </si>
+  <si>
+    <t>Updated On</t>
+  </si>
+  <si>
+    <t>Created On</t>
+  </si>
+  <si>
+    <t>Need to implement search function</t>
   </si>
 </sst>
 </file>
@@ -278,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -307,9 +328,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -622,8 +640,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +676,7 @@
         <v>43</v>
       </c>
       <c r="G1" s="1"/>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>44</v>
       </c>
     </row>
@@ -682,7 +700,7 @@
       <c r="G2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="13"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -698,7 +716,7 @@
         <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F3" s="1">
         <v>11</v>
@@ -706,9 +724,7 @@
       <c r="G3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>45</v>
-      </c>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -726,7 +742,7 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="13"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -748,7 +764,7 @@
       <c r="G5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="13"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -770,7 +786,7 @@
       <c r="G6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="13"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -792,7 +808,7 @@
       <c r="G7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="13"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -814,7 +830,7 @@
       <c r="G8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="13"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -834,7 +850,7 @@
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="13"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -858,9 +874,7 @@
       <c r="G10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="11" t="s">
-        <v>45</v>
-      </c>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -877,7 +891,7 @@
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="13"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -895,7 +909,7 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="13"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -919,7 +933,9 @@
       <c r="G13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="13"/>
+      <c r="H13" s="12" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -959,15 +975,15 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -978,17 +994,42 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1400:E1400"/>
+  <dimension ref="A1:E1400"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="12.85546875" style="5"/>
+    <col min="1" max="1" width="12.85546875" style="5"/>
+    <col min="2" max="2" width="26.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.85546875" style="5"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="1400" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated for Chrome driver and DDAS.Website
</commit_message>
<xml_diff>
--- a/DDAS.Selenium/Testing_Results.xlsx
+++ b/DDAS.Selenium/Testing_Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="DDAS" sheetId="1" r:id="rId1"/>
@@ -195,7 +195,7 @@
     <t>Created On</t>
   </si>
   <si>
-    <t>Need to implement search function</t>
+    <t>Need to implement indexing to search names.</t>
   </si>
 </sst>
 </file>
@@ -640,7 +640,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -996,7 +996,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E1400"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
All sites are in place, working except SAM.
</commit_message>
<xml_diff>
--- a/DDAS.Selenium/Testing_Results.xlsx
+++ b/DDAS.Selenium/Testing_Results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
   <si>
     <t>URL</t>
   </si>
@@ -109,15 +109,6 @@
     <t>Websites used for Due Diligence Process</t>
   </si>
   <si>
-    <t>Page Not Found</t>
-  </si>
-  <si>
-    <t>Unable to figure out what data is to be extracted</t>
-  </si>
-  <si>
-    <t>PAGE NOT FOUND!!</t>
-  </si>
-  <si>
     <t>Has a search box. Last name and first name</t>
   </si>
   <si>
@@ -125,16 +116,6 @@
   </si>
   <si>
     <t>Names Available(Y/N)</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Has a search box. 
-Company name is available but there are no person names</t>
   </si>
   <si>
     <t>Time taken to write each page from PDF:
@@ -196,6 +177,38 @@
   </si>
   <si>
     <t>Need to implement indexing to search names.</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Error handling for NoSuchElementException</t>
+  </si>
+  <si>
+    <t>Click on 'Search Records' button, enter name to search and search the names from the list</t>
+  </si>
+  <si>
+    <t>Search the names directly from the available list</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has a search box. 
+</t>
+  </si>
+  <si>
+    <t>15 Sep 2016: Unable to test this site with PhantomJS driver. Exception - StaleElementReferenceException. Need to look into this</t>
+  </si>
+  <si>
+    <t>Navigate to the website, Click on 'PHS administrative action bulletin board' link and search for names
+Alternate URL: https://ori.hhs.gov/ORI_PHS_alert.html?d=update</t>
+  </si>
+  <si>
+    <t>15 Sep 2016: Update LoadContent function to change the firstname and lastname and search</t>
+  </si>
+  <si>
+    <t>Need to Loop through all records</t>
   </si>
 </sst>
 </file>
@@ -242,7 +255,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -320,12 +333,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -334,6 +341,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -638,10 +651,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,10 +666,11 @@
     <col min="5" max="5" width="42.28515625" customWidth="1"/>
     <col min="6" max="6" width="31.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.85546875" customWidth="1"/>
-    <col min="8" max="8" width="28" customWidth="1"/>
+    <col min="8" max="8" width="31.28515625" customWidth="1"/>
+    <col min="9" max="9" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -667,20 +681,23 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>43</v>
+      <c r="F1" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="G1" s="1"/>
-      <c r="H1" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -691,18 +708,21 @@
         <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1">
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="12"/>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -713,38 +733,48 @@
         <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F3" s="1">
         <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="12"/>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="C4" s="12" t="s">
+        <v>55</v>
+      </c>
       <c r="D4" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="12"/>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H4" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -755,18 +785,21 @@
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1">
         <v>9</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="12"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -777,18 +810,21 @@
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1">
         <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="12"/>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -799,18 +835,21 @@
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1">
         <v>7</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="12"/>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -821,38 +860,44 @@
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
         <v>51</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="12"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>29</v>
+      <c r="C9" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H9" s="10"/>
+      <c r="I9" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -863,55 +908,67 @@
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F10" s="1">
         <v>124</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="12"/>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="C11" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="D11" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="12"/>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H11" s="10"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="12" t="s">
+        <v>55</v>
+      </c>
       <c r="D12" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="12"/>
-    </row>
-    <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H12" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -922,19 +979,22 @@
         <v>4</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F13" s="1">
         <v>56</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>56</v>
+        <v>36</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -975,15 +1035,15 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1007,27 +1067,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="1400" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
SearchSummary updated. Able to find documents by Id (Object Id). Guid has been used.
</commit_message>
<xml_diff>
--- a/DDAS.Selenium/Testing_Results.xlsx
+++ b/DDAS.Selenium/Testing_Results.xlsx
@@ -674,10 +674,10 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="H7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Able to add ClinicalInvestigatorInspectionList data into mongoDB.
</commit_message>
<xml_diff>
--- a/DDAS.Selenium/Testing_Results.xlsx
+++ b/DDAS.Selenium/Testing_Results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="65">
   <si>
     <t>URL</t>
   </si>
@@ -201,17 +201,11 @@
     <t>15 Sep 2016: Update LoadContent function to change the firstname and lastname and search</t>
   </si>
   <si>
-    <t>Error</t>
-  </si>
-  <si>
     <t>Comments on time taken to read records</t>
   </si>
   <si>
     <t>19-Sep-16: Need to find a way to download search results into csv file rather than going through all the records.
 20-Sep-16: Able to loop through all the records But there are new properties found such as, Activation Date, Classification which were not found earlier. New properties were found for the search name 'Hari'</t>
-  </si>
-  <si>
-    <t>21-Sep-16: Need to find a way to bypass the search and download all records at once. Currently going with the web scraping option but need to internally make call to the SAM server ang get the details at one go</t>
   </si>
   <si>
     <t>Need to check for the last updated date in the website</t>
@@ -225,7 +219,12 @@
 27-Sep-16: Connected to mongodb. Able to add extracted records</t>
   </si>
   <si>
-    <t>Adding RowNumber for each record is pending</t>
+    <t>Adding RowNumber is pending</t>
+  </si>
+  <si>
+    <t>21-Sep-16: Need to find a way to bypass the search and download all records at once. Currently going with the web scraping option but need to internally make call to the SAM server ang get the details at one go
+4-Oct-16: Adding RowNumber is pending
+5-Oct-16: Explore the options to download the data from 'Data Access' tab</t>
   </si>
 </sst>
 </file>
@@ -329,7 +328,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -364,9 +363,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -671,13 +667,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="H7" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="D10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,7 +686,7 @@
     <col min="9" max="9" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -713,7 +706,7 @@
         <v>37</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>38</v>
@@ -722,7 +715,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -736,7 +729,7 @@
         <v>30</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F2" s="1">
         <v>4</v>
@@ -745,11 +738,9 @@
         <v>34</v>
       </c>
       <c r="H2" s="10"/>
-      <c r="I2" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -772,12 +763,11 @@
         <v>35</v>
       </c>
       <c r="H3" s="10"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="I3" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -798,10 +788,11 @@
       <c r="H4" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="13"/>
-    </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="I4" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -824,7 +815,7 @@
       <c r="H5" s="10"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -838,7 +829,7 @@
         <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
@@ -849,7 +840,7 @@
       <c r="H6" s="10"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -872,7 +863,7 @@
       <c r="H7" s="10"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -895,7 +886,7 @@
       <c r="H8" s="10"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -909,14 +900,14 @@
         <v>30</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="10"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -941,10 +932,11 @@
       <c r="H10" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="13"/>
-    </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="I10" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -965,7 +957,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -984,13 +976,13 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1016,7 +1008,7 @@
         <v>50</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>